<commit_message>
ear Future Launch Vehicles Support
Added Near Future Launch Vehicles Support with Engine Upgrades; Added Fuel Tank Upgrade to Stock/Restock/NFLV; Added Structural Upgrades to Mk1,Mk2,Mk3 Spaceplane Systems; Added some rescaled parts such as 3.75m and 5m SAS modules; Minor Rebalancing.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDED1208-DDE0-4494-8EC1-F4A8C8C63AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B672C23A-639F-447C-BB47-5DD7999FD6A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15405" yWindow="2160" windowWidth="15075" windowHeight="6975" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-10425" yWindow="240" windowWidth="10050" windowHeight="8895" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="A9:L9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,30 +453,30 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>2150</v>
       </c>
       <c r="C2">
-        <v>820</v>
+        <v>345</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>360</v>
+        <v>2580</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>902.00000000000011</v>
+        <v>379.50000000000006</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
-        <v>20000</v>
+        <v>13500</v>
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>270000</v>
+        <v>133500</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
-        <v>0.60000000000000009</v>
+        <v>0.42500000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -484,18 +484,18 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>40000</v>
+        <v>27000</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>295</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>87.804878048780481</v>
+        <v>2206.086956521739</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>220.00000000000003</v>
+        <v>324.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>180000</v>
+        <v>89000</v>
       </c>
       <c r="C4">
         <v>1E-3</v>
@@ -518,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -538,6 +538,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <f>250/335*18</f>
+        <v>13.432835820895523</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Kerbal Atomics and CryoTanks Support
Added Kerbal Atomics and CryoTanks Support; Modifies tank upgrades depending on CryoTanks installation; Changed color scheme for Engine Switches based on fuel types; Added new tier on Nuclear Propulsion for Kerbal Atomics Upgrades
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B672C23A-639F-447C-BB47-5DD7999FD6A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5CF82-D3C2-4E9F-BC0D-00677CBA080C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10425" yWindow="240" windowWidth="10050" windowHeight="8895" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-13275" yWindow="150" windowWidth="13185" windowHeight="11310" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Thrust</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Added Mass</t>
+  </si>
+  <si>
+    <t>ASL Thrust</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L7" sqref="H7:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,30 +456,30 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2150</v>
+        <v>1950</v>
       </c>
       <c r="C2">
-        <v>345</v>
+        <v>1250</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>2580</v>
+        <v>2340</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>379.50000000000006</v>
+        <v>1375</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
-        <v>13500</v>
+        <v>77500</v>
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>133500</v>
+        <v>442500</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
-        <v>0.42500000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -484,18 +487,18 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>27000</v>
+        <v>155000</v>
       </c>
       <c r="C3">
-        <v>295</v>
+        <v>1170</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>2206.086956521739</v>
+        <v>2190.2400000000002</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>324.5</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -503,14 +506,14 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>89000</v>
+        <v>295000</v>
       </c>
       <c r="C4">
-        <v>1E-3</v>
+        <v>850</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <v>935.00000000000011</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -518,7 +521,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -532,16 +535,19 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <f>C3/C2*B2</f>
+        <v>1825.2</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <f>250/335*18</f>
-        <v>13.432835820895523</v>
-      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Added Cryogenic Engines Support
Added Cryogenic Engines Support
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5CF82-D3C2-4E9F-BC0D-00677CBA080C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B5CEC-ACC8-4354-9931-D7B2732FABBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13275" yWindow="150" windowWidth="13185" windowHeight="11310" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-12015" yWindow="210" windowWidth="11430" windowHeight="11415" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Thrust</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>ASL Thrust</t>
+  </si>
+  <si>
+    <t>Methalox Variant</t>
+  </si>
+  <si>
+    <t>Hydrolox ISP</t>
+  </si>
+  <si>
+    <t>Extended</t>
   </si>
 </sst>
 </file>
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7C98D3-547B-4A15-AC28-017307996FD0}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="H7:L23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,30 +465,30 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1950</v>
+        <v>2850</v>
       </c>
       <c r="C2">
-        <v>1250</v>
+        <v>410</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>2340</v>
+        <v>3420</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>1375</v>
+        <v>451.00000000000006</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
-        <v>77500</v>
+        <v>3150</v>
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>442500</v>
+        <v>142500</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
-        <v>0.60000000000000009</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -487,18 +496,18 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>155000</v>
+        <v>6300</v>
       </c>
       <c r="C3">
-        <v>1170</v>
+        <v>365</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>2190.2400000000002</v>
+        <v>3044.6341463414633</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>1287</v>
+        <v>401.50000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -506,14 +515,14 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>295000</v>
+        <v>95000</v>
       </c>
       <c r="C4">
-        <v>850</v>
+        <v>300</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>935.00000000000011</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -521,11 +530,14 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -540,7 +552,7 @@
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>1825.2</v>
+        <v>2537.1951219512193</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -550,6 +562,139 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>360</v>
+      </c>
+      <c r="C12">
+        <f>0.82*G12</f>
+        <v>383.75999999999993</v>
+      </c>
+      <c r="D12">
+        <f>B12*1.2</f>
+        <v>432</v>
+      </c>
+      <c r="E12">
+        <f>C12*1.1</f>
+        <v>422.13599999999997</v>
+      </c>
+      <c r="G12">
+        <f>H12/1.1</f>
+        <v>467.99999999999994</v>
+      </c>
+      <c r="H12">
+        <v>514.79999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>(C13/C12)*B12</f>
+        <v>96.153846153846146</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C18" si="1">0.82*G13</f>
+        <v>102.49999999999999</v>
+      </c>
+      <c r="D13">
+        <f>(E13/E12)*D12</f>
+        <v>115.38461538461539</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E18" si="2">C13*1.1</f>
+        <v>112.75</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G15" si="3">H13/1.1</f>
+        <v>124.99999999999999</v>
+      </c>
+      <c r="H13">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>20.499999999999996</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>22.549999999999997</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>24.999999999999996</v>
+      </c>
+      <c r="H14">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>9.02</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Near Future Aeronautics Support
Added Near Future Aeronautics Support; Removed the Needs CommunityTechTree from some parts (felt redundant).  Moved Experimental Aircraft Engines to alternative propulsion branch; Added new node in aeronautics branch, one in flight systems, one in alternate propulsion.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A1590-D4CE-4A5F-B741-3CAA94355B7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF61164-102B-44D1-ACC9-1478E8F6AC5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22215" yWindow="2010" windowWidth="14655" windowHeight="7605" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-15540" yWindow="7170" windowWidth="14655" windowHeight="8415" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Thrust</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Extended</t>
+  </si>
+  <si>
+    <t>10 Atm</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,18 +468,18 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>264</v>
+        <v>700</v>
       </c>
       <c r="C2">
-        <v>470</v>
+        <v>345</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>316.8</v>
+        <v>840</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>517</v>
+        <v>379.50000000000006</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
@@ -484,7 +487,7 @@
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>252000</v>
+        <v>450000</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
@@ -499,15 +502,15 @@
         <v>6300</v>
       </c>
       <c r="C3">
-        <v>399.8</v>
+        <v>225</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>269.48221276595746</v>
+        <v>547.82608695652175</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>439.78000000000003</v>
+        <v>247.50000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -515,14 +518,14 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>168000</v>
+        <v>300000</v>
       </c>
       <c r="C4">
-        <v>290</v>
+        <v>120</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>319</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -533,17 +536,24 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <f>(C5/C2)*D2</f>
+        <v>97.391304347826093</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>220.00000000000003</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>1E-3</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -552,7 +562,7 @@
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>224.56851063829788</v>
+        <v>456.52173913043481</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -560,6 +570,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>C5/C2*B2</f>
+        <v>81.159420289855078</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Luciole and Modular Launch Pads Support
Added Luciole and Modular Launch Pads Support; Changed the color of RealPlume engine support indicator in part descriptions; fixed typo in 0.625 rescaled monoprop parts; Shifted KOOSE parts to re-entry module branch; Stock solar patches for Near Future Solar in an earlier pass.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF61164-102B-44D1-ACC9-1478E8F6AC5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7444DF4E-7F55-41B5-8AEB-DE6E7A2669B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15540" yWindow="7170" windowWidth="14655" windowHeight="8415" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-28515" yWindow="2175" windowWidth="15660" windowHeight="10755" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,18 +468,18 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>700</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>840</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>379.50000000000006</v>
+        <v>374.00000000000006</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
@@ -487,7 +487,7 @@
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>450000</v>
+        <v>5400</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
@@ -502,15 +502,15 @@
         <v>6300</v>
       </c>
       <c r="C3">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>547.82608695652175</v>
+        <v>9.3176470588235283</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>247.50000000000003</v>
+        <v>242.00000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -518,14 +518,14 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>300000</v>
+        <v>3600</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -536,15 +536,15 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="D5">
         <f>(C5/C2)*D2</f>
-        <v>97.391304347826093</v>
+        <v>5.2941176470588234</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -562,7 +562,7 @@
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>456.52173913043481</v>
+        <v>7.764705882352942</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="B8">
         <f>C5/C2*B2</f>
-        <v>81.159420289855078</v>
+        <v>4.4117647058823533</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
James Webb, Deep Space Surface Habitat Unit, Making Alternate History, and Duna Direct Support
Added James Webb, Deep Space Surface Habitat Unit, Making Alternate History, and Duna Direct Support; Increased the additional mass for upgraded engines to 10% from 5%; Fixed Typos in Mk1-3 Part Upgrade Text
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7444DF4E-7F55-41B5-8AEB-DE6E7A2669B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339A8AE0-4463-4AA3-B653-928D8409E987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28515" yWindow="2175" windowWidth="15660" windowHeight="10755" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-10020" yWindow="240" windowWidth="10020" windowHeight="13200" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,26 +468,26 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>14.399999999999999</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <f>C2*1.1</f>
-        <v>374.00000000000006</v>
+        <v>387.20000000000005</v>
       </c>
       <c r="F2">
         <f>B3*0.5</f>
-        <v>3150</v>
+        <v>2500</v>
       </c>
       <c r="G2">
         <f>B4*1.5</f>
-        <v>5400</v>
+        <v>4500</v>
       </c>
       <c r="H2">
         <f>0.05*B5</f>
@@ -499,18 +499,18 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>6300</v>
+        <v>5000</v>
       </c>
       <c r="C3">
-        <v>220</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>9.3176470588235283</v>
+        <v>1.7045454545454544</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>242.00000000000003</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -518,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>3600</v>
+        <v>3000</v>
       </c>
       <c r="C4">
         <v>1E-3</v>
@@ -536,15 +536,15 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>125</v>
+        <v>1E-3</v>
       </c>
       <c r="D5">
         <f>(C5/C2)*D2</f>
-        <v>5.2941176470588234</v>
+        <v>8.5227272727272734E-5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>137.5</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -562,7 +562,7 @@
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>7.764705882352942</v>
+        <v>1.4204545454545454</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="B8">
         <f>C5/C2*B2</f>
-        <v>4.4117647058823533</v>
+        <v>7.1022727272727283E-5</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -601,26 +601,26 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>360</v>
+        <v>80</v>
       </c>
       <c r="C12">
         <f>0.82*G12</f>
-        <v>385.39999999999992</v>
+        <v>367.35999999999996</v>
       </c>
       <c r="D12">
         <f>B12*1.2</f>
-        <v>432</v>
+        <v>96</v>
       </c>
       <c r="E12">
         <f>C12*1.1</f>
-        <v>423.93999999999994</v>
+        <v>404.096</v>
       </c>
       <c r="G12">
         <f>H12/1.1</f>
-        <v>469.99999999999994</v>
+        <v>448</v>
       </c>
       <c r="H12">
-        <v>517</v>
+        <v>492.8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -629,60 +629,60 @@
       </c>
       <c r="B13">
         <f>(C13/C12)*B12</f>
-        <v>306.22978723404259</v>
+        <v>17.857142857142854</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:C18" si="1">0.82*G13</f>
-        <v>327.83599999999996</v>
+        <v>81.999999999999986</v>
       </c>
       <c r="D13">
         <f>(E13/E12)*D12</f>
-        <v>367.47574468085111</v>
+        <v>21.428571428571423</v>
       </c>
       <c r="E13">
         <f t="shared" ref="E13:E18" si="2">C13*1.1</f>
-        <v>360.61959999999999</v>
+        <v>90.199999999999989</v>
       </c>
       <c r="G13">
         <f t="shared" ref="G13:G16" si="3">H13/1.1</f>
-        <v>399.79999999999995</v>
+        <v>99.999999999999986</v>
       </c>
       <c r="H13">
-        <v>439.78</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>237.79999999999998</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>261.58</v>
+        <v>18.04</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>290</v>
+        <v>20</v>
       </c>
       <c r="H14">
-        <v>319</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>7.4545454545454541E-3</v>
+        <v>7.4545454545454546E-4</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>8.2000000000000007E-3</v>
+        <v>8.2000000000000009E-4</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>9.0909090909090905E-3</v>
+        <v>9.0909090909090909E-4</v>
       </c>
       <c r="H15">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
MK2 Stockalike Expansion Support
Added MK2 Stockalike Expansion Support; Slight tweak of Moroz; Fixed bug that Mk2-3 LF/O tanks had access to multiple upgrades when CryoTanks installed; Moved MkIV crew cabin to same branch as cockpit.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D9B01-62D2-4818-938A-BD502C7D7B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BF6915-A6EF-4FE3-AD40-66AF163368FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9735" yWindow="0" windowWidth="9450" windowHeight="15600" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-13530" yWindow="570" windowWidth="13530" windowHeight="9240" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Thrust</t>
   </si>
@@ -44,9 +44,6 @@
     <t>20% Thrust</t>
   </si>
   <si>
-    <t>10% Efficiency</t>
-  </si>
-  <si>
     <t>Engine</t>
   </si>
   <si>
@@ -81,6 +78,12 @@
   </si>
   <si>
     <t>10 Atm</t>
+  </si>
+  <si>
+    <t>10% Effic</t>
+  </si>
+  <si>
+    <t>30% Effic</t>
   </si>
 </sst>
 </file>
@@ -432,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7C98D3-547B-4A15-AC28-017307996FD0}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -451,74 +454,85 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2">
-        <v>270</v>
+        <v>190</v>
       </c>
       <c r="C2">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>324</v>
+        <v>228</v>
       </c>
       <c r="E2">
-        <f>C2*1.1</f>
-        <v>394.90000000000003</v>
+        <f>$C2*1.1</f>
+        <v>379.50000000000006</v>
       </c>
       <c r="F2">
+        <f>$C2*1.3</f>
+        <v>448.5</v>
+      </c>
+      <c r="G2">
         <f>B3*0.5</f>
-        <v>2500</v>
-      </c>
-      <c r="G2">
+        <v>4750</v>
+      </c>
+      <c r="H2">
         <f>B4*1.5</f>
-        <v>11250</v>
-      </c>
-      <c r="H2">
+        <v>33000</v>
+      </c>
+      <c r="I2">
         <f>0.05*B5</f>
         <v>0.15000000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>5000</v>
+        <v>9500</v>
       </c>
       <c r="C3">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>108.30083565459609</v>
+        <v>59.478260869565219</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">C3*1.1</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E3:F8" si="0">$C3*1.1</f>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="1">$C3*1.3</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>7500</v>
+        <v>22000</v>
       </c>
       <c r="C4">
         <v>1E-3</v>
@@ -527,27 +541,35 @@
         <f t="shared" si="0"/>
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1E-3</v>
+        <v>150</v>
       </c>
       <c r="D5">
         <f>(C5/C2)*D2</f>
-        <v>9.0250696378830087E-4</v>
+        <v>99.130434782608688</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>1E-3</v>
       </c>
@@ -555,56 +577,68 @@
         <f t="shared" si="0"/>
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>90.250696378830085</v>
+        <v>49.565217391304344</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <f>C5/C2*B2</f>
-        <v>7.5208913649025069E-4</v>
+        <v>82.608695652173907</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>80</v>
       </c>
       <c r="C12">
-        <f>0.82*G12</f>
+        <f>0.82*H12</f>
         <v>367.35999999999996</v>
       </c>
       <c r="D12">
@@ -615,24 +649,24 @@
         <f>C12*1.1</f>
         <v>404.096</v>
       </c>
-      <c r="G12">
-        <f>H12/1.1</f>
+      <c r="H12">
+        <f>I12/1.1</f>
         <v>448</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>492.8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <f>(C13/C12)*B12</f>
         <v>17.857142857142854</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C18" si="1">0.82*G13</f>
+        <f t="shared" ref="C13:C18" si="2">0.82*H13</f>
         <v>81.999999999999986</v>
       </c>
       <c r="D13">
@@ -640,82 +674,82 @@
         <v>21.428571428571423</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E18" si="2">C13*1.1</f>
+        <f t="shared" ref="E13:E18" si="3">C13*1.1</f>
         <v>90.199999999999989</v>
       </c>
-      <c r="G13">
-        <f t="shared" ref="G13:G16" si="3">H13/1.1</f>
+      <c r="H13">
+        <f t="shared" ref="H13:H16" si="4">I13/1.1</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.399999999999999</v>
       </c>
       <c r="E14">
+        <f t="shared" si="3"/>
+        <v>18.04</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C15">
         <f t="shared" si="2"/>
-        <v>18.04</v>
-      </c>
-      <c r="G14">
+        <v>7.4545454545454546E-4</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>7.4545454545454546E-4</v>
-      </c>
-      <c r="E15">
+        <v>8.2000000000000009E-4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>9.0909090909090909E-4</v>
+      </c>
+      <c r="I15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C16">
         <f t="shared" si="2"/>
-        <v>8.2000000000000009E-4</v>
-      </c>
-      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="3"/>
-        <v>9.0909090909090909E-4</v>
-      </c>
-      <c r="H15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MK3 Stockalike Expansion and Kerbal Reusability Expansion Support
Added MK3 Stockalike Expansion and Kerbal Reusability Expansion Support; Moved RoveMax Model XL3 one tier earlier in tech tree; Moved some AirplanePlus parts a touch earlier in the tech tree; Moved the decoupling and docking ports for Mk2 Stockalike Expansion
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BF6915-A6EF-4FE3-AD40-66AF163368FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B0898C-4199-4D30-A04F-FC3DA92395D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13530" yWindow="570" windowWidth="13530" windowHeight="9240" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-12795" yWindow="150" windowWidth="12660" windowHeight="9240" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,22 +474,22 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>190</v>
+        <v>480</v>
       </c>
       <c r="C2">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D2">
         <f>B2*1.2</f>
-        <v>228</v>
+        <v>576</v>
       </c>
       <c r="E2">
         <f>$C2*1.1</f>
-        <v>379.50000000000006</v>
+        <v>374.00000000000006</v>
       </c>
       <c r="F2">
         <f>$C2*1.3</f>
-        <v>448.5</v>
+        <v>442</v>
       </c>
       <c r="G2">
         <f>B3*0.5</f>
@@ -497,7 +497,7 @@
       </c>
       <c r="H2">
         <f>B4*1.5</f>
-        <v>33000</v>
+        <v>240000</v>
       </c>
       <c r="I2">
         <f>0.05*B5</f>
@@ -512,19 +512,19 @@
         <v>9500</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>290</v>
       </c>
       <c r="D3">
         <f>(E3/E2)*D2</f>
-        <v>59.478260869565219</v>
+        <v>491.29411764705873</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:F8" si="0">$C3*1.1</f>
-        <v>99.000000000000014</v>
+        <f t="shared" ref="E3:E8" si="0">$C3*1.1</f>
+        <v>319</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" si="1">$C3*1.3</f>
-        <v>117</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -532,18 +532,18 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>22000</v>
+        <v>160000</v>
       </c>
       <c r="C4">
-        <v>1E-3</v>
+        <v>230</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <v>253.00000000000003</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>1.3000000000000002E-3</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -554,19 +554,19 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D5">
         <f>(C5/C2)*D2</f>
-        <v>99.130434782608688</v>
+        <v>288</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>187.00000000000003</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -588,7 +588,7 @@
       </c>
       <c r="B7">
         <f>C3/C2*B2</f>
-        <v>49.565217391304344</v>
+        <v>409.41176470588232</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -605,7 +605,7 @@
       </c>
       <c r="B8">
         <f>C5/C2*B2</f>
-        <v>82.608695652173907</v>
+        <v>240</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
BonVoyage, Decoupler Shroud, Dodo Labs, kOS, SmartParts, and The Martian for KSP Support
Added BonVoyage, Decoupler Shroud, Dodo Labs, kOS, SmartParts, and The Martian for KSP Support; Lowered entry cost of Calypso engine in Knes; Fixed tech node for Multi-Role Kapsule DM in Knes; Added parachute upgrade support for KOOSE, Bumblebee, and Fuji; Added B9 Plural to Cryotanks patch (Fuel Mixes, copied from The Martian for KSP by bcink); Moved cubesats from Luciole to Unkerballed Tech and increased cost.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BD6495-C138-4E08-94BC-A1C5EDFC687E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31516069-73A2-4D1F-BC53-EEEF7B264B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11565" yWindow="45" windowWidth="5145" windowHeight="5760" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-11190" yWindow="105" windowWidth="11190" windowHeight="13230" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,26 +494,26 @@
         <v>3</v>
       </c>
       <c r="B2" s="4">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4">
-        <v>260</v>
+        <v>340</v>
       </c>
       <c r="D2" s="3">
         <f>B2*1.2</f>
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E2" s="3">
         <f>$C2*1.1</f>
-        <v>286</v>
+        <v>374.00000000000006</v>
       </c>
       <c r="F2" s="3">
         <f>$C2*1.3</f>
-        <v>338</v>
+        <v>442</v>
       </c>
       <c r="G2">
         <f>B3*1.5</f>
-        <v>5250</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -521,22 +521,22 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>3500</v>
+        <v>15000</v>
       </c>
       <c r="C3" s="4">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="D3" s="3">
         <f>(E3/E2)*D2</f>
-        <v>73.5</v>
+        <v>57.882352941176464</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E8" si="0">$C3*1.1</f>
-        <v>269.5</v>
+        <v>225.50000000000003</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F8" si="1">$C3*1.3</f>
-        <v>318.5</v>
+        <v>266.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -559,7 +559,7 @@
       </c>
       <c r="D5" s="3">
         <f>(C5/C2)*D2</f>
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="B7" s="3">
         <f>C3/C2*B2</f>
-        <v>61.25</v>
+        <v>48.235294117647058</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="B8" s="3">
         <f>C5/C2*B2</f>
-        <v>42.5</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -640,19 +640,19 @@
       </c>
       <c r="B11" s="3">
         <f>B2*1.08</f>
-        <v>70.2</v>
+        <v>86.4</v>
       </c>
       <c r="C11">
         <f>C2*1.3</f>
-        <v>338</v>
+        <v>442</v>
       </c>
       <c r="D11">
         <f>B11*1.2</f>
-        <v>84.24</v>
+        <v>103.68</v>
       </c>
       <c r="E11">
         <f>C11*1.1</f>
-        <v>371.8</v>
+        <v>486.20000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -661,19 +661,19 @@
       </c>
       <c r="B12" s="3">
         <f>(C12/C11)*B11</f>
-        <v>66.150000000000006</v>
+        <v>52.094117647058823</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C15" si="2">C3*1.3</f>
-        <v>318.5</v>
+        <v>266.5</v>
       </c>
       <c r="D12">
         <f>B12*1.2</f>
-        <v>79.38000000000001</v>
+        <v>62.512941176470584</v>
       </c>
       <c r="E12">
         <f t="shared" ref="E12:E15" si="3">C12*1.1</f>
-        <v>350.35</v>
+        <v>293.15000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -748,23 +748,23 @@
       </c>
       <c r="B20" s="3">
         <f>IF(I20&lt;&gt;"",I20,B11)</f>
-        <v>70.2</v>
+        <v>86.4</v>
       </c>
       <c r="C20" s="3">
         <f>0.82*G20</f>
-        <v>277.15999999999997</v>
+        <v>362.44</v>
       </c>
       <c r="D20" s="3">
         <f>B20*1.2</f>
-        <v>84.24</v>
+        <v>103.68</v>
       </c>
       <c r="E20" s="3">
         <f>C20*1.1</f>
-        <v>304.87599999999998</v>
+        <v>398.68400000000003</v>
       </c>
       <c r="G20">
         <f>IF(H20&lt;&gt;"",H20/1.1,C11)</f>
-        <v>338</v>
+        <v>442</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -775,23 +775,23 @@
       </c>
       <c r="B21" s="3">
         <f>(C21/C20)*B20</f>
-        <v>66.150000000000006</v>
+        <v>52.094117647058823</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" ref="C21:C26" si="4">0.82*G21</f>
-        <v>261.16999999999996</v>
+        <v>218.53</v>
       </c>
       <c r="D21" s="3">
         <f>(E21/E20)*D20</f>
-        <v>79.38</v>
+        <v>62.512941176470591</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ref="E21:E26" si="5">C21*1.1</f>
-        <v>287.28699999999998</v>
+        <v>240.38300000000001</v>
       </c>
       <c r="G21">
         <f>IF(H21&lt;&gt;"",H21/1.1,C12)</f>
-        <v>318.5</v>
+        <v>266.5</v>
       </c>
       <c r="H21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Mandatory RCS and Kerbal GPS Revived Support
Mandatory RCS and Kerbal GPS Revived Support; Added MonoPropellant Engine Upgrades to Internal RCS, Knes, Mk2 Stockalike Expansion, Mk3 Stockalike Expansion, Near Future Spacecraft; and Stock;  Fixed 0 cost for STEAM Blamont MonoPropellant Module in Knes.
</commit_message>
<xml_diff>
--- a/Source/EngineUpgrade.xlsx
+++ b/Source/EngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3623A75C-1AE1-48E1-B52B-80048A7C0E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E36B367-055B-490C-A4DF-E6BB4A072387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12030" yWindow="0" windowWidth="11805" windowHeight="12390" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
+    <workbookView xWindow="-15120" yWindow="360" windowWidth="14625" windowHeight="11895" xr2:uid="{2C8768AD-A958-4913-8B06-1EC1F27AC2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,26 +494,26 @@
         <v>15</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
+        <v>560</v>
       </c>
       <c r="C2" s="4">
-        <v>240</v>
+        <v>337</v>
       </c>
       <c r="D2" s="3">
         <f>B2*1.2</f>
-        <v>4.8</v>
+        <v>672</v>
       </c>
       <c r="E2" s="3">
         <f>$C2*1.1</f>
-        <v>264</v>
+        <v>370.70000000000005</v>
       </c>
       <c r="F2" s="3">
         <f>$C2*1.3</f>
-        <v>312</v>
+        <v>438.1</v>
       </c>
       <c r="G2">
         <f>B7*1.5</f>
-        <v>1350</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -522,22 +522,22 @@
       </c>
       <c r="B3" s="3">
         <f>C3/C2*B2</f>
-        <v>2</v>
+        <v>353.94658753709194</v>
       </c>
       <c r="C3" s="4">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="D3" s="3">
         <f>(E3/E2)*D2</f>
-        <v>2.4</v>
+        <v>424.73590504451033</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E6" si="0">$C3*1.1</f>
-        <v>132</v>
+        <v>234.3</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F6" si="1">$C3*1.3</f>
-        <v>156</v>
+        <v>276.90000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -592,7 +592,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>900</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -618,19 +618,19 @@
       </c>
       <c r="B11" s="3">
         <f>B2*1.08</f>
-        <v>4.32</v>
+        <v>604.80000000000007</v>
       </c>
       <c r="C11">
         <f>C2*1.3</f>
-        <v>312</v>
+        <v>438.1</v>
       </c>
       <c r="D11">
         <f>B11*1.2</f>
-        <v>5.1840000000000002</v>
+        <v>725.7600000000001</v>
       </c>
       <c r="E11">
         <f>C11*1.1</f>
-        <v>343.20000000000005</v>
+        <v>481.91000000000008</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -639,19 +639,19 @@
       </c>
       <c r="B12" s="3">
         <f>(C12/C11)*B11</f>
-        <v>2.16</v>
+        <v>382.26231454005944</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C15" si="2">C3*1.3</f>
-        <v>156</v>
+        <v>276.90000000000003</v>
       </c>
       <c r="D12">
         <f>B12*1.2</f>
-        <v>2.5920000000000001</v>
+        <v>458.71477744807129</v>
       </c>
       <c r="E12">
         <f t="shared" ref="E12:E15" si="3">C12*1.1</f>
-        <v>171.60000000000002</v>
+        <v>304.59000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -733,23 +733,23 @@
       </c>
       <c r="B20" s="3">
         <f>IF(I20&lt;&gt;"",I20,B11)</f>
-        <v>4.32</v>
+        <v>604.80000000000007</v>
       </c>
       <c r="C20" s="3">
         <f>0.82*G20</f>
-        <v>255.83999999999997</v>
+        <v>359.24200000000002</v>
       </c>
       <c r="D20" s="3">
         <f>B20*1.2</f>
-        <v>5.1840000000000002</v>
+        <v>725.7600000000001</v>
       </c>
       <c r="E20" s="3">
         <f>C20*1.1</f>
-        <v>281.42399999999998</v>
+        <v>395.16620000000006</v>
       </c>
       <c r="G20">
         <f>IF(H20&lt;&gt;"",H20/1.1,C11)</f>
-        <v>312</v>
+        <v>438.1</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -760,23 +760,23 @@
       </c>
       <c r="B21" s="3">
         <f>(C21/C20)*B20</f>
-        <v>2.16</v>
+        <v>382.26231454005944</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" ref="C21:C24" si="4">0.82*G21</f>
-        <v>127.91999999999999</v>
+        <v>227.05800000000002</v>
       </c>
       <c r="D21" s="3">
         <f>(E21/E20)*D20</f>
-        <v>2.5920000000000001</v>
+        <v>458.71477744807123</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ref="E21:E24" si="5">C21*1.1</f>
-        <v>140.71199999999999</v>
+        <v>249.76380000000003</v>
       </c>
       <c r="G21">
         <f>IF(H21&lt;&gt;"",H21/1.1,C12)</f>
-        <v>156</v>
+        <v>276.90000000000003</v>
       </c>
       <c r="H21" s="1"/>
     </row>

</xml_diff>